<commit_message>
Fixing typos and adding a Sync for setting number of employees
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
+++ b/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t>TestScenario</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t>Show 20 employees on table</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -682,8 +694,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1467,14 +1480,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1495,8 +1507,8 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>5</v>
+      <c r="C2" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1506,8 +1518,8 @@
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>10</v>
+      <c r="C3" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1517,8 +1529,8 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>15</v>
+      <c r="C4" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1528,8 +1540,8 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>20</v>
+      <c r="C5" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworded stories to make more shorthand
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
+++ b/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="SearchForEmployees" sheetId="1" r:id="rId1"/>
     <sheet name="SearchEmployeeTableColumns" sheetId="2" r:id="rId2"/>
-    <sheet name="ShowEmployeesPerPage" sheetId="3" r:id="rId3"/>
+    <sheet name="SortEmployeeTableColumns" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1480,7 +1480,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Removed extra datarow and changed to run on Firefox
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
+++ b/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t>TestScenario</t>
   </si>
@@ -1190,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1220,13 +1220,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1243,26 +1243,26 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1271,26 +1271,26 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -1299,26 +1299,26 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1327,26 +1327,26 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1355,26 +1355,26 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1383,26 +1383,26 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -1411,26 +1411,26 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -1439,26 +1439,26 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -1467,20 +1467,6 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed scenarios for Sorting Test as some scenarios would take too long to validate
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
+++ b/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>TestScenario</t>
   </si>
@@ -143,46 +143,28 @@
     <t>Sort by Last Name on the Employee Page in Descending Order</t>
   </si>
   <si>
-    <t>Sort by Title on the Employee Page in Ascending Order</t>
-  </si>
-  <si>
     <t>Sort by Title on the Employee Page in Descending Order</t>
   </si>
   <si>
     <t>Sort by Supervisor on the Employee Page in Ascending Order</t>
   </si>
   <si>
-    <t>Sort by Supervisor on the Employee Page in Descending Order</t>
-  </si>
-  <si>
     <t>Sort by Project on the Employee Page in Ascending Order</t>
   </si>
   <si>
     <t>Sort by Project on the Employee Page in Descending Order</t>
   </si>
   <si>
-    <t>Sort by Location on the Employee Page in Ascending Order</t>
-  </si>
-  <si>
     <t>Sort by Location on the Employee Page in Descending Order</t>
   </si>
   <si>
     <t>Sort by Vacation Days Left on the Employee Page in Ascending Order</t>
   </si>
   <si>
-    <t>Sort by Vacation Days Left on the Employee Page in Descending Order</t>
-  </si>
-  <si>
     <t>Sort by Sick Days Left on the Employee Page in Ascending Order</t>
   </si>
   <si>
-    <t>Sort by Sick Days Left on the Employee Page in Descending Order</t>
-  </si>
-  <si>
     <t>Sort by Floating Days Left on the Employee Page in Ascending Order</t>
-  </si>
-  <si>
-    <t>Sort by Floating Days Left on the Employee Page in Descending Order</t>
   </si>
   <si>
     <t>EmployeesPerPage</t>
@@ -1190,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,7 +1267,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1296,10 +1278,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1310,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -1324,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -1338,10 +1320,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1352,10 +1334,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1366,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>31</v>
@@ -1380,94 +1362,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1497,51 +1395,51 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feature MAnageEmployee-AddEmployee. Created Employee class to store data
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
+++ b/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SearchForEmployees" sheetId="1" r:id="rId1"/>
     <sheet name="SortEmployeeTableColumns" sheetId="2" r:id="rId2"/>
     <sheet name="ShowEmployeesPerPage" sheetId="3" r:id="rId3"/>
+    <sheet name="FilterEmployees" sheetId="4" r:id="rId4"/>
+    <sheet name="AddEmployee" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
   <si>
     <t>TestScenario</t>
   </si>
@@ -192,6 +194,12 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>Filter Employees on Employee Page as Company Admin</t>
+  </si>
+  <si>
+    <t>Add New Employee as Company Admin</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1035,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1174,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1445,4 +1453,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="47.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated core, added new tests
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
+++ b/src/test/resources/bluesource/dataProviders/ManageEmployees.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980"/>
   </bookViews>
   <sheets>
     <sheet name="SearchForEmployees" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>TestScenario</t>
   </si>
@@ -67,18 +67,12 @@
     <t>LASTNAME</t>
   </si>
   <si>
-    <t>FirstEmployee</t>
-  </si>
-  <si>
     <t>FIRSTNAME</t>
   </si>
   <si>
     <t>Love</t>
   </si>
   <si>
-    <t>Software Consultant</t>
-  </si>
-  <si>
     <t>TITLE</t>
   </si>
   <si>
@@ -94,12 +88,6 @@
     <t>Search for Location on Employee Page as Company Admin</t>
   </si>
   <si>
-    <t>Adam Thomas</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
     <t>SUPERVISOR</t>
   </si>
   <si>
@@ -109,9 +97,6 @@
     <t>LOCATION</t>
   </si>
   <si>
-    <t>Watchdogs</t>
-  </si>
-  <si>
     <t>SortColumn</t>
   </si>
   <si>
@@ -200,6 +185,24 @@
   </si>
   <si>
     <t>Add New Employee as Company Admin</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Greensboro</t>
+  </si>
+  <si>
+    <t>Bluesource</t>
+  </si>
+  <si>
+    <t>Kristi</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Perry Thomas</t>
   </si>
 </sst>
 </file>
@@ -1034,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1068,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -1082,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1110,66 +1113,66 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1202,43 +1205,43 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1247,12 +1250,12 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1261,119 +1264,119 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1403,51 +1406,51 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1479,7 +1482,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -1494,7 +1497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1512,7 +1517,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>

</xml_diff>